<commit_message>
Tests to be rewritten
</commit_message>
<xml_diff>
--- a/ifc_to_openroads/data/WSDOT_Item_Types.xlsx
+++ b/ifc_to_openroads/data/WSDOT_Item_Types.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMITHS4\Python Projects\ifcCreator\IFC Table Extraction\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMITHS4\Python Projects\ifcCreator\ifc_to_openroads\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F267B4A-047A-42B3-BAA2-BF43C2C135D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300F50ED-62E6-4052-B1B1-41FB3556E7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5265" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="5112" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Library</t>
   </si>
@@ -113,40 +113,7 @@
     <t>73274</t>
   </si>
   <si>
-    <t>PERMANENT SIGNING</t>
-  </si>
-  <si>
-    <t>6890</t>
-  </si>
-  <si>
-    <t>L.S.</t>
-  </si>
-  <si>
-    <t>D10-2</t>
-  </si>
-  <si>
-    <t>Reference Location Signs (miles)</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Guide</t>
-  </si>
-  <si>
-    <t>U.S. 2004</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ()</t>
-  </si>
-  <si>
-    <t>Install</t>
-  </si>
-  <si>
-    <t>TRAFFIC</t>
   </si>
 </sst>
 </file>
@@ -520,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,41 +599,8 @@
       <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="T2" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>